<commit_message>
adds queries from Jeanine created may 17 2023
</commit_message>
<xml_diff>
--- a/data-raw/metadata/camp_metadata.xlsx
+++ b/data-raw/metadata/camp_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/jpe-knights-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FC66012-1A68-CA4D-9E82-4E625DEA499F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1F77418-37E6-9F42-AC70-2BF01B9E87ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33580" yWindow="2120" windowWidth="30240" windowHeight="17200" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset" sheetId="1" r:id="rId1"/>
@@ -280,9 +280,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -306,12 +306,6 @@
       <color rgb="FF494A4C"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
     </font>
     <font>
       <u/>
@@ -367,7 +361,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -388,15 +382,15 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -16750,7 +16744,7 @@
       <c r="B2" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="11" t="s">
         <v>65</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -16768,7 +16762,7 @@
       <c r="B3" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="11" t="s">
         <v>64</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -51052,7 +51046,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -51089,7 +51083,7 @@
       </c>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="14" t="s">
         <v>68</v>
       </c>
       <c r="B2">
@@ -51104,10 +51098,10 @@
       <c r="E2">
         <v>38.802278000000001</v>
       </c>
-      <c r="F2" s="13">
+      <c r="F2" s="12">
         <v>38992</v>
       </c>
-      <c r="G2" s="14">
+      <c r="G2" s="13">
         <v>44699</v>
       </c>
       <c r="H2" s="7"/>
@@ -51131,22 +51125,22 @@
       <c r="Z2" s="7"/>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G3" s="11"/>
+      <c r="G3" s="10"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G4" s="11"/>
+      <c r="G4" s="10"/>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G5" s="11"/>
+      <c r="G5" s="10"/>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G6" s="11"/>
+      <c r="G6" s="10"/>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G7" s="11"/>
+      <c r="G7" s="10"/>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G8" s="11"/>
+      <c r="G8" s="10"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>